<commit_message>
Updates template for CE04OSSM and creates R00001
</commit_message>
<xml_diff>
--- a/CE04OSSM/CE04OSSM_R0000#_ingest.xlsx
+++ b/CE04OSSM/CE04OSSM_R0000#_ingest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="CE04OSSM_R0000#_ingest_v#" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
   <si>
     <t>uframe_route</t>
   </si>
@@ -85,87 +85,36 @@
     <t>Ingest.wavss-a-dcl_recovered</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl11/mopak_*/*.mopak.log</t>
-  </si>
-  <si>
-    <t>CE04OSSM-SBD11-01-MOPAKO000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/metbk1_*/*.metbk*.log </t>
-  </si>
-  <si>
     <t>CE04OSSM-SBD11-06-METBKA000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl11/velpt1_*/*.velpt*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-SBD11-04-VELPTA000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl26/velpt2_*/*.velpt*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID26-04-VELPTA000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/pco2a_*/PCO2A*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-SBD12-04-PCO2AA000</t>
   </si>
   <si>
-    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/wavss_*/*.wavss.log </t>
-  </si>
-  <si>
     <t>CE04OSSM-SBD12-05-WAVSSA000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/adcpt_*/*adcpt.log</t>
-  </si>
-  <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl26/PHSEN_*/SAMI*.txt</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID26-06-PHSEND000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/OPTAA_*/*.optaa*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID27-01-OPTAAD000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/FLORT_*/*.flort.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID27-02-FLORTD000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/CTDBP_*/*ctdbp*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID27-03-CTDBPC000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/DOSTA_*/*dosta*.log</t>
-  </si>
-  <si>
     <t>CE04OSSM-RID27-04-DOSTAD000</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/NUTNR_*/*SCH*.DAT</t>
-  </si>
-  <si>
-    <t>CE04OSSM-RID27-07-NUTNRB000</t>
-  </si>
-  <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/spkir_*/*.spkir*.log</t>
-  </si>
-  <si>
-    <t>CE04OSSM-RID27-08-SPKIRB000</t>
-  </si>
-  <si>
     <t>Note:  Change the file name to uniquely identify it; i.e., CE04OSSM_R0000#_ingest_v#; where R0000# identifies deployment number, and v# identifies the version of this document.</t>
   </si>
   <si>
@@ -202,12 +151,6 @@
     <t>Ingest.cg-dcl-eng-dcl_recovered</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/irid2shore/cpm_status*.txt</t>
-  </si>
-  <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/cpm2/syslog/cpm_status*.txt</t>
-  </si>
-  <si>
     <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/syslog/*.syslog.log</t>
   </si>
   <si>
@@ -217,17 +160,92 @@
     <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/syslog/*.syslog.log</t>
   </si>
   <si>
-    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/dcl27/syslog/*.syslog.log</t>
-  </si>
-  <si>
     <t>Ingest.ctdbp-cdef-cp_recovered</t>
+  </si>
+  <si>
+    <t>This is a single file updated every minute. There will only be 1 of these files and the data in it will be from the last update.</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/cpm2/syslog/cpm_status.txt</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/mopak/*.mopak.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/wavss/*.wavss.log </t>
+  </si>
+  <si>
+    <t>CE04OSSM-RID26-07-NUTNRB000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-RID26-08-SPKIRB000</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/pco2a/*.pco2a.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/metbk/*.metbk.log </t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl27/syslog/*.syslog.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/irid2shore/cpm_status*.txt</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl27/dosta/*.dosta.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl27/flort/*.flort.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl27/optaa/*.optaa.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/spkir/*.spkir.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/phsen/*.phsen.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/hyd1/*.hyd1.log</t>
+  </si>
+  <si>
+    <t>Ingest.hyd-o-dcl_recovered</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/hyd2/*.hyd2.log</t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD12-03-HYDGN0000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD11-02-HYDGN0000</t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD11-01-MOPAK0000</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl11/VELPT_*/*velpt*.aqd</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl26/ADCPT_*/*adcpt*.pd0</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl26/VELPT_*/*velpt*.aqd</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl26/NUTNR_*/*nutnr*/*SCH*.DAT</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl27/CTDBP_*/*ctdbp*.hex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,13 +380,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1248833</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1291167</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -409,13 +427,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2466976</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2550584</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>42333</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -530,7 +548,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -565,7 +582,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -741,16 +757,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="525" activePane="bottomLeft"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="81.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -759,7 +771,7 @@
     <col min="5" max="5" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -773,422 +785,462 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75">
+      <c r="A3" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75">
+      <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75">
+      <c r="A6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75">
+      <c r="A8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="12"/>
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75">
+      <c r="A10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75">
+      <c r="A14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75">
+      <c r="A15" s="12"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="D21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="D25" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="45">
+      <c r="A28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24"/>
-      <c r="B24"/>
-      <c r="C24"/>
-      <c r="D24"/>
-      <c r="E24"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25"/>
-      <c r="B25"/>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26"/>
-      <c r="B26"/>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28"/>
-      <c r="B28"/>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30"/>
-      <c r="B30" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32"/>
-      <c r="B32" s="8" t="s">
-        <v>17</v>
-      </c>
+    <row r="32" spans="1:6">
+      <c r="A32" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="8"/>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32"/>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7">
       <c r="A35"/>
-      <c r="B35"/>
+      <c r="B35" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7">
       <c r="A36"/>
-      <c r="B36" s="11"/>
+      <c r="B36"/>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
+    <row r="37" spans="1:7">
+      <c r="A37"/>
+      <c r="B37" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41"/>
+      <c r="B41" s="11"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="4"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates RNNNNN templates for Endurance and creates new RNNNNN .csv sheets
</commit_message>
<xml_diff>
--- a/CE04OSSM/CE04OSSM_R0000#_ingest.xlsx
+++ b/CE04OSSM/CE04OSSM_R0000#_ingest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405"/>
+    <workbookView xWindow="-15" yWindow="6435" windowWidth="28860" windowHeight="6495"/>
   </bookViews>
   <sheets>
     <sheet name="CE04OSSM_R0000#_ingest_v#" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t>uframe_route</t>
   </si>
@@ -118,15 +118,9 @@
     <t>Note:  Change the file name to uniquely identify it; i.e., CE04OSSM_R0000#_ingest_v#; where R0000# identifies deployment number, and v# identifies the version of this document.</t>
   </si>
   <si>
-    <t>CE04OSSM-RID26-01-ADCPTC000</t>
-  </si>
-  <si>
     <t>Ingest.adcpt-acfgm-dcl-pd0_recovered</t>
   </si>
   <si>
-    <t>Ingest.nutnr-b-dcl-full_recovered</t>
-  </si>
-  <si>
     <t>CE04OSSM-SBC11-00-CPMENG000</t>
   </si>
   <si>
@@ -239,6 +233,66 @@
   </si>
   <si>
     <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl27/CTDBP_*/*ctdbp*.hex</t>
+  </si>
+  <si>
+    <t>Ingest.velpt-ab-dcl_recovered</t>
+  </si>
+  <si>
+    <t>Recovered DCL data</t>
+  </si>
+  <si>
+    <t>Recovered Instrument data</t>
+  </si>
+  <si>
+    <t>Ingest.fdchp-a-dcl_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.fdchp-a_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.adcps-jln_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.phsen-abcdef_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.nutnr-b-dcl-conc_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.nutnr-b_recovered</t>
+  </si>
+  <si>
+    <t>Ingest.ctdbp-cdef-dcl-cp_recovered</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl11/velpt1/*.velpt1.log</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl12/fdchp/*.fdchp.log </t>
+  </si>
+  <si>
+    <t>CE04OSSM-SBD12-08-FDCHPA000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl12/FDCHP_*/*fdchp*/fdchp*.dat </t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/adcpt/*.adcpt.log</t>
+  </si>
+  <si>
+    <t>CE04OSSM-RID26-01-ADCPTA000</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/velpt2/*.velpt2.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/instrmts/dcl26/PHSEN_*/*phsen*.txt</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl26/nutnr/*.nutnr.log</t>
+  </si>
+  <si>
+    <t>/omc_data/whoi/OMC/CE04OSSM/R00001/cg_data/dcl27/ctdbp/*.ctdbp.log</t>
   </si>
 </sst>
 </file>
@@ -380,13 +434,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1248833</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1291167</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>158750</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -427,13 +481,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2466976</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2550584</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>42333</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -758,9 +812,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -790,10 +846,10 @@
         <v>14</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -801,24 +857,24 @@
     </row>
     <row r="3" spans="1:5" ht="15.75">
       <c r="A3" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
+    <row r="4" spans="1:5" ht="15.75">
+      <c r="A4" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>
@@ -826,347 +882,453 @@
       <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75">
-      <c r="A5" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>52</v>
+      <c r="E4" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75">
       <c r="A6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75">
+      <c r="A7" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1" t="s">
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75">
-      <c r="A8" s="12" t="s">
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75">
+      <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B9" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75">
-      <c r="A9" s="12"/>
-      <c r="B9" s="14"/>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75">
-      <c r="A10" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="A10" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75">
+      <c r="A11" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75">
+      <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="4" t="s">
-        <v>6</v>
-      </c>
       <c r="B12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>83</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
+      <c r="E12" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75">
+      <c r="A13" s="15" t="s">
+        <v>74</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75">
       <c r="A14" s="12" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75">
-      <c r="A15" s="12"/>
+      <c r="E14" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75">
+      <c r="A20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="4" t="s">
+      <c r="D21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B22" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="16" t="s">
+      <c r="C27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="17" t="s">
+      <c r="C28" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="D28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" s="17" t="s">
+      <c r="D29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23"/>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="17" t="s">
+      <c r="D30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25"/>
-    </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26"/>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="45">
-      <c r="A28" s="6" t="s">
+      <c r="D31" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="45">
+      <c r="A33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29"/>
-      <c r="B29"/>
-      <c r="C29"/>
-      <c r="D29"/>
-      <c r="E29"/>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30"/>
-      <c r="B30"/>
-      <c r="C30"/>
-      <c r="D30"/>
-      <c r="E30"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31"/>
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:7">
       <c r="A34"/>
@@ -1177,9 +1339,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35"/>
-      <c r="B35" s="9" t="s">
-        <v>13</v>
-      </c>
+      <c r="B35"/>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
@@ -1192,15 +1352,13 @@
       <c r="E36"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37"/>
-      <c r="B37" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A37" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="8"/>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
+      <c r="E37"/>
     </row>
     <row r="38" spans="1:7">
       <c r="A38"/>
@@ -1218,29 +1376,70 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40"/>
-      <c r="B40"/>
+      <c r="B40" s="9" t="s">
+        <v>13</v>
+      </c>
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
     </row>
     <row r="41" spans="1:7">
       <c r="A41"/>
-      <c r="B41" s="11"/>
+      <c r="B41"/>
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="4"/>
+      <c r="A42"/>
+      <c r="B42" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="4"/>
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="4"/>
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="4"/>
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46"/>
+      <c r="B46" s="11"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>